<commit_message>
changes to the rolling window forecast and the output simulation
</commit_message>
<xml_diff>
--- a/Prefered_PARX_model_forecast/Resultater_PAR/KLIC_PAR.xlsx
+++ b/Prefered_PARX_model_forecast/Resultater_PAR/KLIC_PAR.xlsx
@@ -28,7 +28,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -38,14 +38,22 @@
     </border>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -58,7 +66,7 @@
   <dimension ref="A1:A464"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="true"/>
+    <col min="1" max="1" width="14.42578125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -668,1717 +676,1717 @@
     </row>
     <row r="122">
       <c r="A122">
-        <v>-1.2029496039500969</v>
+        <v>-1.2029499037569247</v>
       </c>
     </row>
     <row r="123">
       <c r="A123">
-        <v>-1.0273217925769305</v>
+        <v>-1.0273220772407652</v>
       </c>
     </row>
     <row r="124">
       <c r="A124">
-        <v>-1.0727649839815059</v>
+        <v>-1.0727651040812614</v>
       </c>
     </row>
     <row r="125">
       <c r="A125">
-        <v>-1.0512581889525046</v>
+        <v>-1.0512583396622397</v>
       </c>
     </row>
     <row r="126">
       <c r="A126">
-        <v>-1.2318460553021597</v>
+        <v>-1.2318460220707206</v>
       </c>
     </row>
     <row r="127">
       <c r="A127">
-        <v>-0.892895749976783</v>
+        <v>-0.89289570599945101</v>
       </c>
     </row>
     <row r="128">
       <c r="A128">
-        <v>-0.78987493692881217</v>
+        <v>-0.7898748849357905</v>
       </c>
     </row>
     <row r="129">
       <c r="A129">
-        <v>-0.75156538038912779</v>
+        <v>-0.75156537791483613</v>
       </c>
     </row>
     <row r="130">
       <c r="A130">
-        <v>-0.75081297102294209</v>
+        <v>-0.75081296577405054</v>
       </c>
     </row>
     <row r="131">
       <c r="A131">
-        <v>-0.84841281745872732</v>
+        <v>-0.84841291546368003</v>
       </c>
     </row>
     <row r="132">
       <c r="A132">
-        <v>-0.64974988031504977</v>
+        <v>-0.64974997055263062</v>
       </c>
     </row>
     <row r="133">
       <c r="A133">
-        <v>-0.42598641070402898</v>
+        <v>-0.42598642659254654</v>
       </c>
     </row>
     <row r="134">
       <c r="A134">
-        <v>-0.38238452922618699</v>
+        <v>-0.38238453573118786</v>
       </c>
     </row>
     <row r="135">
       <c r="A135">
-        <v>-0.35463176396955715</v>
+        <v>-0.35463171987526321</v>
       </c>
     </row>
     <row r="136">
       <c r="A136">
-        <v>-0.34315724134927944</v>
+        <v>-0.34315721191070275</v>
       </c>
     </row>
     <row r="137">
       <c r="A137">
-        <v>-0.3728995880634185</v>
+        <v>-0.3728995575425848</v>
       </c>
     </row>
     <row r="138">
       <c r="A138">
-        <v>-0.43818011429922266</v>
+        <v>-0.43818008139396775</v>
       </c>
     </row>
     <row r="139">
       <c r="A139">
-        <v>-0.44416216639755718</v>
+        <v>-0.44416214856430658</v>
       </c>
     </row>
     <row r="140">
       <c r="A140">
-        <v>-0.46213939090966943</v>
+        <v>-0.46213937874725719</v>
       </c>
     </row>
     <row r="141">
       <c r="A141">
-        <v>-0.47798611647774336</v>
+        <v>-0.4779860778440651</v>
       </c>
     </row>
     <row r="142">
       <c r="A142">
-        <v>-0.44023428626171951</v>
+        <v>-0.44023424665001321</v>
       </c>
     </row>
     <row r="143">
       <c r="A143">
-        <v>-0.44788074840439718</v>
+        <v>-0.44788071004136359</v>
       </c>
     </row>
     <row r="144">
       <c r="A144">
-        <v>-0.474892206952719</v>
+        <v>-0.47489217561768676</v>
       </c>
     </row>
     <row r="145">
       <c r="A145">
-        <v>-0.37842467254448231</v>
+        <v>-0.37842456343198649</v>
       </c>
     </row>
     <row r="146">
       <c r="A146">
-        <v>-0.4238179927612179</v>
+        <v>-0.42381789766584171</v>
       </c>
     </row>
     <row r="147">
       <c r="A147">
-        <v>-0.47828185002180384</v>
+        <v>-0.47828180479344135</v>
       </c>
     </row>
     <row r="148">
       <c r="A148">
-        <v>-0.38731067264101021</v>
+        <v>-0.38731059981732796</v>
       </c>
     </row>
     <row r="149">
       <c r="A149">
-        <v>-0.31525014120737066</v>
+        <v>-0.31525008708606211</v>
       </c>
     </row>
     <row r="150">
       <c r="A150">
-        <v>-0.3066667715389953</v>
+        <v>-0.30666671636155823</v>
       </c>
     </row>
     <row r="151">
       <c r="A151">
-        <v>-0.31234339904183911</v>
+        <v>-0.31234337164855247</v>
       </c>
     </row>
     <row r="152">
       <c r="A152">
-        <v>-0.3180200544955103</v>
+        <v>-0.31802003821579283</v>
       </c>
     </row>
     <row r="153">
       <c r="A153">
-        <v>-0.33316840519865687</v>
+        <v>-0.33316839576928448</v>
       </c>
     </row>
     <row r="154">
       <c r="A154">
-        <v>-0.34253132039754475</v>
+        <v>-0.34253124498666654</v>
       </c>
     </row>
     <row r="155">
       <c r="A155">
-        <v>-0.374080446169685</v>
+        <v>-0.37408037401637739</v>
       </c>
     </row>
     <row r="156">
       <c r="A156">
-        <v>-0.40973596647895261</v>
+        <v>-0.40973588164646385</v>
       </c>
     </row>
     <row r="157">
       <c r="A157">
-        <v>-0.42616443860637271</v>
+        <v>-0.42616435599499358</v>
       </c>
     </row>
     <row r="158">
       <c r="A158">
-        <v>-0.47300385871683348</v>
+        <v>-0.4730038030401566</v>
       </c>
     </row>
     <row r="159">
       <c r="A159">
-        <v>-0.49876768245102371</v>
+        <v>-0.49876766883680684</v>
       </c>
     </row>
     <row r="160">
       <c r="A160">
-        <v>-0.51550865966902171</v>
+        <v>-0.51550864554183817</v>
       </c>
     </row>
     <row r="161">
       <c r="A161">
-        <v>-0.56514196672029315</v>
+        <v>-0.56514193228277287</v>
       </c>
     </row>
     <row r="162">
       <c r="A162">
-        <v>-0.55401896167466913</v>
+        <v>-0.55401892566888844</v>
       </c>
     </row>
     <row r="163">
       <c r="A163">
-        <v>-0.52144545710514112</v>
+        <v>-0.52144542822532891</v>
       </c>
     </row>
     <row r="164">
       <c r="A164">
-        <v>-0.34089834382902845</v>
+        <v>-0.34089834918239298</v>
       </c>
     </row>
     <row r="165">
       <c r="A165">
-        <v>-0.16046663486471313</v>
+        <v>-0.16046664791083137</v>
       </c>
     </row>
     <row r="166">
       <c r="A166">
-        <v>-0.054121714231612265</v>
+        <v>-0.054121716070341087</v>
       </c>
     </row>
     <row r="167">
       <c r="A167">
-        <v>0.0088310934472141094</v>
+        <v>0.0088311129704604467</v>
       </c>
     </row>
     <row r="168">
       <c r="A168">
-        <v>0.16246513767169254</v>
+        <v>0.16246513408906219</v>
       </c>
     </row>
     <row r="169">
       <c r="A169">
-        <v>0.4540388310712265</v>
+        <v>0.45403878891781063</v>
       </c>
     </row>
     <row r="170">
       <c r="A170">
-        <v>0.67987576910234726</v>
+        <v>0.67987572442507915</v>
       </c>
     </row>
     <row r="171">
       <c r="A171">
-        <v>1.0294171032051656</v>
+        <v>1.029417037454843</v>
       </c>
     </row>
     <row r="172">
       <c r="A172">
-        <v>1.2241419353440097</v>
+        <v>1.2241418754776057</v>
       </c>
     </row>
     <row r="173">
       <c r="A173">
-        <v>1.4471327295948402</v>
+        <v>1.4471326164964962</v>
       </c>
     </row>
     <row r="174">
       <c r="A174">
-        <v>1.7062847919451516</v>
+        <v>1.7062846829845912</v>
       </c>
     </row>
     <row r="175">
       <c r="A175">
-        <v>2.157573940517155</v>
+        <v>2.1575738618661613</v>
       </c>
     </row>
     <row r="176">
       <c r="A176">
-        <v>2.4315352723353856</v>
+        <v>2.4315351872754136</v>
       </c>
     </row>
     <row r="177">
       <c r="A177">
-        <v>2.6815526591865981</v>
+        <v>2.6815526079861516</v>
       </c>
     </row>
     <row r="178">
       <c r="A178">
-        <v>3.1772831153558405</v>
+        <v>3.177282988066692</v>
       </c>
     </row>
     <row r="179">
       <c r="A179">
-        <v>3.6267797014613055</v>
+        <v>3.6267795821193602</v>
       </c>
     </row>
     <row r="180">
       <c r="A180">
-        <v>4.1006095628317496</v>
+        <v>4.1006094578815588</v>
       </c>
     </row>
     <row r="181">
       <c r="A181">
-        <v>4.3570373170679852</v>
+        <v>4.3570372065017837</v>
       </c>
     </row>
     <row r="182">
       <c r="A182">
-        <v>4.8217506653777003</v>
+        <v>4.8217504960624344</v>
       </c>
     </row>
     <row r="183">
       <c r="A183">
-        <v>5.4306760611832336</v>
+        <v>5.4306758687856647</v>
       </c>
     </row>
     <row r="184">
       <c r="A184">
-        <v>5.8031231420632441</v>
+        <v>5.8031229537876472</v>
       </c>
     </row>
     <row r="185">
       <c r="A185">
-        <v>5.9539460782545461</v>
+        <v>5.9539459053325272</v>
       </c>
     </row>
     <row r="186">
       <c r="A186">
-        <v>6.2189140095748581</v>
+        <v>6.2189138217130422</v>
       </c>
     </row>
     <row r="187">
       <c r="A187">
-        <v>6.5780741777222271</v>
+        <v>6.578074019638346</v>
       </c>
     </row>
     <row r="188">
       <c r="A188">
-        <v>6.766492203117223</v>
+        <v>6.7664920224194054</v>
       </c>
     </row>
     <row r="189">
       <c r="A189">
-        <v>7.0516948399345694</v>
+        <v>7.0516946378661807</v>
       </c>
     </row>
     <row r="190">
       <c r="A190">
-        <v>7.4450135452602373</v>
+        <v>7.4450133736888997</v>
       </c>
     </row>
     <row r="191">
       <c r="A191">
-        <v>7.7560578782462857</v>
+        <v>7.7560577270229709</v>
       </c>
     </row>
     <row r="192">
       <c r="A192">
-        <v>7.8391507858205376</v>
+        <v>7.8391506251065941</v>
       </c>
     </row>
     <row r="193">
       <c r="A193">
-        <v>8.076597403136212</v>
+        <v>8.0765972402364543</v>
       </c>
     </row>
     <row r="194">
       <c r="A194">
-        <v>8.5975755557469142</v>
+        <v>8.5975753321536601</v>
       </c>
     </row>
     <row r="195">
       <c r="A195">
-        <v>8.6543453712219058</v>
+        <v>8.6543451479832125</v>
       </c>
     </row>
     <row r="196">
       <c r="A196">
-        <v>8.7878251666206459</v>
+        <v>8.7878249598988578</v>
       </c>
     </row>
     <row r="197">
       <c r="A197">
-        <v>8.7918582290995388</v>
+        <v>8.7918580104901292</v>
       </c>
     </row>
     <row r="198">
       <c r="A198">
-        <v>8.8606417620611087</v>
+        <v>8.8606415198836554</v>
       </c>
     </row>
     <row r="199">
       <c r="A199">
-        <v>8.9636877453039343</v>
+        <v>8.9636874579777093</v>
       </c>
     </row>
     <row r="200">
       <c r="A200">
-        <v>9.0533226855754148</v>
+        <v>9.0533223961512075</v>
       </c>
     </row>
     <row r="201">
       <c r="A201">
-        <v>9.3121667974126279</v>
+        <v>9.3121665190051761</v>
       </c>
     </row>
     <row r="202">
       <c r="A202">
-        <v>9.5472803214442568</v>
+        <v>9.5472800425287616</v>
       </c>
     </row>
     <row r="203">
       <c r="A203">
-        <v>9.8261972067210746</v>
+        <v>9.8261969085745875</v>
       </c>
     </row>
     <row r="204">
       <c r="A204">
-        <v>10.093858266435138</v>
+        <v>10.093857945503736</v>
       </c>
     </row>
     <row r="205">
       <c r="A205">
-        <v>10.353142379181167</v>
+        <v>10.353142084113493</v>
       </c>
     </row>
     <row r="206">
       <c r="A206">
-        <v>10.478750909932169</v>
+        <v>10.478750603560918</v>
       </c>
     </row>
     <row r="207">
       <c r="A207">
-        <v>10.738871403938058</v>
+        <v>10.738871056640804</v>
       </c>
     </row>
     <row r="208">
       <c r="A208">
-        <v>11.072405102485817</v>
+        <v>11.072404696906451</v>
       </c>
     </row>
     <row r="209">
       <c r="A209">
-        <v>11.286517653755142</v>
+        <v>11.286517237435634</v>
       </c>
     </row>
     <row r="210">
       <c r="A210">
-        <v>11.589804193060225</v>
+        <v>11.589803726007649</v>
       </c>
     </row>
     <row r="211">
       <c r="A211">
-        <v>11.769161812846537</v>
+        <v>11.769161364223102</v>
       </c>
     </row>
     <row r="212">
       <c r="A212">
-        <v>12.088656059259094</v>
+        <v>12.088655637943791</v>
       </c>
     </row>
     <row r="213">
       <c r="A213">
-        <v>12.348873296795807</v>
+        <v>12.34887291069848</v>
       </c>
     </row>
     <row r="214">
       <c r="A214">
-        <v>12.688643040019464</v>
+        <v>12.688642639390793</v>
       </c>
     </row>
     <row r="215">
       <c r="A215">
-        <v>13.154156487938348</v>
+        <v>13.154156128655227</v>
       </c>
     </row>
     <row r="216">
       <c r="A216">
-        <v>13.720064386587195</v>
+        <v>13.720063992429166</v>
       </c>
     </row>
     <row r="217">
       <c r="A217">
-        <v>14.187354584689286</v>
+        <v>14.187354248477298</v>
       </c>
     </row>
     <row r="218">
       <c r="A218">
-        <v>14.784617667590137</v>
+        <v>14.784617320406605</v>
       </c>
     </row>
     <row r="219">
       <c r="A219">
-        <v>15.313239278106868</v>
+        <v>15.313238810484838</v>
       </c>
     </row>
     <row r="220">
       <c r="A220">
-        <v>15.980255125869203</v>
+        <v>15.980254616775182</v>
       </c>
     </row>
     <row r="221">
       <c r="A221">
-        <v>16.625327025488588</v>
+        <v>16.625326488911263</v>
       </c>
     </row>
     <row r="222">
       <c r="A222">
-        <v>17.304273604539244</v>
+        <v>17.304273074036303</v>
       </c>
     </row>
     <row r="223">
       <c r="A223">
-        <v>18.004811016479238</v>
+        <v>18.004810538352899</v>
       </c>
     </row>
     <row r="224">
       <c r="A224">
-        <v>18.964640064717663</v>
+        <v>18.964639584975341</v>
       </c>
     </row>
     <row r="225">
       <c r="A225">
-        <v>19.876517393903416</v>
+        <v>19.876516988686166</v>
       </c>
     </row>
     <row r="226">
       <c r="A226">
-        <v>20.361804087872535</v>
+        <v>20.361803691764518</v>
       </c>
     </row>
     <row r="227">
       <c r="A227">
-        <v>20.716325614326589</v>
+        <v>20.716325218368709</v>
       </c>
     </row>
     <row r="228">
       <c r="A228">
-        <v>21.243774305384356</v>
+        <v>21.24377396698199</v>
       </c>
     </row>
     <row r="229">
       <c r="A229">
-        <v>22.179748557836106</v>
+        <v>22.179748233229713</v>
       </c>
     </row>
     <row r="230">
       <c r="A230">
-        <v>22.754042335413143</v>
+        <v>22.754042016263803</v>
       </c>
     </row>
     <row r="231">
       <c r="A231">
-        <v>23.535320300225152</v>
+        <v>23.535319986308004</v>
       </c>
     </row>
     <row r="232">
       <c r="A232">
-        <v>23.997049682353708</v>
+        <v>23.997049323820882</v>
       </c>
     </row>
     <row r="233">
       <c r="A233">
-        <v>24.511665322057883</v>
+        <v>24.511664975423077</v>
       </c>
     </row>
     <row r="234">
       <c r="A234">
-        <v>24.918055669702078</v>
+        <v>24.918055313056126</v>
       </c>
     </row>
     <row r="235">
       <c r="A235">
-        <v>25.258737332576086</v>
+        <v>25.258736989908886</v>
       </c>
     </row>
     <row r="236">
       <c r="A236">
-        <v>25.930255022350199</v>
+        <v>25.930254724482879</v>
       </c>
     </row>
     <row r="237">
       <c r="A237">
-        <v>26.97450089904935</v>
+        <v>26.974500813257666</v>
       </c>
     </row>
     <row r="238">
       <c r="A238">
-        <v>27.706976454099738</v>
+        <v>27.706976411863408</v>
       </c>
     </row>
     <row r="239">
       <c r="A239">
-        <v>28.292900086190702</v>
+        <v>28.292900058174315</v>
       </c>
     </row>
     <row r="240">
       <c r="A240">
-        <v>28.840418370068921</v>
+        <v>28.840418377305809</v>
       </c>
     </row>
     <row r="241">
       <c r="A241">
-        <v>29.163161906395413</v>
+        <v>29.163161914344176</v>
       </c>
     </row>
     <row r="242">
       <c r="A242">
-        <v>29.598603146073987</v>
+        <v>29.59860310776936</v>
       </c>
     </row>
     <row r="243">
       <c r="A243">
-        <v>30.205554918134499</v>
+        <v>30.205554920792178</v>
       </c>
     </row>
     <row r="244">
       <c r="A244">
-        <v>30.662106710018325</v>
+        <v>30.662106692302928</v>
       </c>
     </row>
     <row r="245">
       <c r="A245">
-        <v>31.244934082661253</v>
+        <v>31.244934011779705</v>
       </c>
     </row>
     <row r="246">
       <c r="A246">
-        <v>31.866858924254228</v>
+        <v>31.866858936094786</v>
       </c>
     </row>
     <row r="247">
       <c r="A247">
-        <v>32.123519680300667</v>
+        <v>32.123519652284365</v>
       </c>
     </row>
     <row r="248">
       <c r="A248">
-        <v>32.349002710121937</v>
+        <v>32.349002692209567</v>
       </c>
     </row>
     <row r="249">
       <c r="A249">
-        <v>32.609078915063449</v>
+        <v>32.609078870562918</v>
       </c>
     </row>
     <row r="250">
       <c r="A250">
-        <v>33.062624590427333</v>
+        <v>33.062624576676555</v>
       </c>
     </row>
     <row r="251">
       <c r="A251">
-        <v>33.657371732975903</v>
+        <v>33.657371668953132</v>
       </c>
     </row>
     <row r="252">
       <c r="A252">
-        <v>34.362112798953667</v>
+        <v>34.362112747566847</v>
       </c>
     </row>
     <row r="253">
       <c r="A253">
-        <v>35.088620338378171</v>
+        <v>35.088620230049507</v>
       </c>
     </row>
     <row r="254">
       <c r="A254">
-        <v>35.834659522247804</v>
+        <v>35.834659534172822</v>
       </c>
     </row>
     <row r="255">
       <c r="A255">
-        <v>36.801994634861643</v>
+        <v>36.801994583928256</v>
       </c>
     </row>
     <row r="256">
       <c r="A256">
-        <v>37.874697064386211</v>
+        <v>37.874696953235166</v>
       </c>
     </row>
     <row r="257">
       <c r="A257">
-        <v>39.421959026209436</v>
+        <v>39.42195891467945</v>
       </c>
     </row>
     <row r="258">
       <c r="A258">
-        <v>40.411401007253339</v>
+        <v>40.411400919807342</v>
       </c>
     </row>
     <row r="259">
       <c r="A259">
-        <v>41.623022677262519</v>
+        <v>41.623022726344473</v>
       </c>
     </row>
     <row r="260">
       <c r="A260">
-        <v>43.380354855446463</v>
+        <v>43.38035492648698</v>
       </c>
     </row>
     <row r="261">
       <c r="A261">
-        <v>45.123547201351982</v>
+        <v>45.123547252965508</v>
       </c>
     </row>
     <row r="262">
       <c r="A262">
-        <v>46.619167500646988</v>
+        <v>46.619167564834207</v>
       </c>
     </row>
     <row r="263">
       <c r="A263">
-        <v>48.474812918804126</v>
+        <v>48.474812936722159</v>
       </c>
     </row>
     <row r="264">
       <c r="A264">
-        <v>50.913717333674761</v>
+        <v>50.913717490109327</v>
       </c>
     </row>
     <row r="265">
       <c r="A265">
-        <v>53.949293058645182</v>
+        <v>53.949293322771098</v>
       </c>
     </row>
     <row r="266">
       <c r="A266">
-        <v>56.959733078274866</v>
+        <v>56.959733411352516</v>
       </c>
     </row>
     <row r="267">
       <c r="A267">
-        <v>60.103859600853021</v>
+        <v>60.103859817566324</v>
       </c>
     </row>
     <row r="268">
       <c r="A268">
-        <v>63.286165423034042</v>
+        <v>63.286165653514303</v>
       </c>
     </row>
     <row r="269">
       <c r="A269">
-        <v>66.544122667823757</v>
+        <v>66.544123045301035</v>
       </c>
     </row>
     <row r="270">
       <c r="A270">
-        <v>69.118794906213253</v>
+        <v>69.118795292923494</v>
       </c>
     </row>
     <row r="271">
       <c r="A271">
-        <v>72.997289542434046</v>
+        <v>72.997289895606997</v>
       </c>
     </row>
     <row r="272">
       <c r="A272">
-        <v>76.040902012997506</v>
+        <v>76.04090244570267</v>
       </c>
     </row>
     <row r="273">
       <c r="A273">
-        <v>79.097753836376341</v>
+        <v>79.097754114058475</v>
       </c>
     </row>
     <row r="274">
       <c r="A274">
-        <v>81.349531067336983</v>
+        <v>81.349531419476463</v>
       </c>
     </row>
     <row r="275">
       <c r="A275">
-        <v>84.602714936557575</v>
+        <v>84.602715332778402</v>
       </c>
     </row>
     <row r="276">
       <c r="A276">
-        <v>87.343006248953387</v>
+        <v>87.343006674528652</v>
       </c>
     </row>
     <row r="277">
       <c r="A277">
-        <v>89.860829716063137</v>
+        <v>89.860830325066729</v>
       </c>
     </row>
     <row r="278">
       <c r="A278">
-        <v>94.040632767688308</v>
+        <v>94.040633402731359</v>
       </c>
     </row>
     <row r="279">
       <c r="A279">
-        <v>96.758385785507699</v>
+        <v>96.758386444366224</v>
       </c>
     </row>
     <row r="280">
       <c r="A280">
-        <v>98.911044374451876</v>
+        <v>98.911044969067746</v>
       </c>
     </row>
     <row r="281">
       <c r="A281">
-        <v>100.8222244195058</v>
+        <v>100.82222498853858</v>
       </c>
     </row>
     <row r="282">
       <c r="A282">
-        <v>103.32408978681784</v>
+        <v>103.32409027237965</v>
       </c>
     </row>
     <row r="283">
       <c r="A283">
-        <v>105.61853891664524</v>
+        <v>105.61853960757027</v>
       </c>
     </row>
     <row r="284">
       <c r="A284">
-        <v>107.35274403573216</v>
+        <v>107.35274470257579</v>
       </c>
     </row>
     <row r="285">
       <c r="A285">
-        <v>109.92154292451232</v>
+        <v>109.92154362742724</v>
       </c>
     </row>
     <row r="286">
       <c r="A286">
-        <v>111.37505195505069</v>
+        <v>111.3750527327693</v>
       </c>
     </row>
     <row r="287">
       <c r="A287">
-        <v>113.20404211550671</v>
+        <v>113.20404292636034</v>
       </c>
     </row>
     <row r="288">
       <c r="A288">
-        <v>115.27424035464719</v>
+        <v>115.27424115565397</v>
       </c>
     </row>
     <row r="289">
       <c r="A289">
-        <v>116.88752999823484</v>
+        <v>116.88753067177258</v>
       </c>
     </row>
     <row r="290">
       <c r="A290">
-        <v>118.35288853552561</v>
+        <v>118.3528892010585</v>
       </c>
     </row>
     <row r="291">
       <c r="A291">
-        <v>119.65390872568597</v>
+        <v>119.65390948323339</v>
       </c>
     </row>
     <row r="292">
       <c r="A292">
-        <v>121.23777167053834</v>
+        <v>121.2377725109499</v>
       </c>
     </row>
     <row r="293">
       <c r="A293">
-        <v>122.31352559223259</v>
+        <v>122.31352645964142</v>
       </c>
     </row>
     <row r="294">
       <c r="A294">
-        <v>123.501087558808</v>
+        <v>123.50108831765337</v>
       </c>
     </row>
     <row r="295">
       <c r="A295">
-        <v>124.33216554238862</v>
+        <v>124.33216645293757</v>
       </c>
     </row>
     <row r="296">
       <c r="A296">
-        <v>125.31960231250932</v>
+        <v>125.31960325016803</v>
       </c>
     </row>
     <row r="297">
       <c r="A297">
-        <v>125.93697029798663</v>
+        <v>125.93697122635271</v>
       </c>
     </row>
     <row r="298">
       <c r="A298">
-        <v>126.52532709712624</v>
+        <v>126.52532809189567</v>
       </c>
     </row>
     <row r="299">
       <c r="A299">
-        <v>127.88956779887374</v>
+        <v>127.8895687909436</v>
       </c>
     </row>
     <row r="300">
       <c r="A300">
-        <v>129.01172200786323</v>
+        <v>129.01172302149499</v>
       </c>
     </row>
     <row r="301">
       <c r="A301">
-        <v>129.37307969753201</v>
+        <v>129.37308072617816</v>
       </c>
     </row>
     <row r="302">
       <c r="A302">
-        <v>130.04890041117477</v>
+        <v>130.04890141464324</v>
       </c>
     </row>
     <row r="303">
       <c r="A303">
-        <v>130.60794518161899</v>
+        <v>130.60794613583073</v>
       </c>
     </row>
     <row r="304">
       <c r="A304">
-        <v>130.77582528637856</v>
+        <v>130.77582614186574</v>
       </c>
     </row>
     <row r="305">
       <c r="A305">
-        <v>130.91403816007966</v>
+        <v>130.91403896991631</v>
       </c>
     </row>
     <row r="306">
       <c r="A306">
-        <v>131.23749125260201</v>
+        <v>131.23749207176363</v>
       </c>
     </row>
     <row r="307">
       <c r="A307">
-        <v>131.22477076710479</v>
+        <v>131.22477162667761</v>
       </c>
     </row>
     <row r="308">
       <c r="A308">
-        <v>131.29305316508336</v>
+        <v>131.29305401093418</v>
       </c>
     </row>
     <row r="309">
       <c r="A309">
-        <v>131.26339123457106</v>
+        <v>131.26339211149735</v>
       </c>
     </row>
     <row r="310">
       <c r="A310">
-        <v>131.17713142366745</v>
+        <v>131.17713234190842</v>
       </c>
     </row>
     <row r="311">
       <c r="A311">
-        <v>130.8179446267759</v>
+        <v>130.81794554091962</v>
       </c>
     </row>
     <row r="312">
       <c r="A312">
-        <v>130.57770778046853</v>
+        <v>130.57770868783192</v>
       </c>
     </row>
     <row r="313">
       <c r="A313">
-        <v>130.43313217505025</v>
+        <v>130.43313308262432</v>
       </c>
     </row>
     <row r="314">
       <c r="A314">
-        <v>130.16792806386374</v>
+        <v>130.16792899042872</v>
       </c>
     </row>
     <row r="315">
       <c r="A315">
-        <v>129.83809739616979</v>
+        <v>129.83809834062467</v>
       </c>
     </row>
     <row r="316">
       <c r="A316">
-        <v>129.49791996348196</v>
+        <v>129.49792092421023</v>
       </c>
     </row>
     <row r="317">
       <c r="A317">
-        <v>129.23647766969623</v>
+        <v>129.23647865396933</v>
       </c>
     </row>
     <row r="318">
       <c r="A318">
-        <v>128.78099513644435</v>
+        <v>128.78099611078289</v>
       </c>
     </row>
     <row r="319">
       <c r="A319">
-        <v>128.39861928468019</v>
+        <v>128.3986202263448</v>
       </c>
     </row>
     <row r="320">
       <c r="A320">
-        <v>128.08497100383195</v>
+        <v>128.08497189892083</v>
       </c>
     </row>
     <row r="321">
       <c r="A321">
-        <v>127.84858599620651</v>
+        <v>127.84858691037647</v>
       </c>
     </row>
     <row r="322">
       <c r="A322">
-        <v>127.58746799798342</v>
+        <v>127.58746891492768</v>
       </c>
     </row>
     <row r="323">
       <c r="A323">
-        <v>127.17369820580045</v>
+        <v>127.17369915787845</v>
       </c>
     </row>
     <row r="324">
       <c r="A324">
-        <v>126.73298016919789</v>
+        <v>126.73298111351728</v>
       </c>
     </row>
     <row r="325">
       <c r="A325">
-        <v>126.38926477753638</v>
+        <v>126.38926573206112</v>
       </c>
     </row>
     <row r="326">
       <c r="A326">
-        <v>125.95340446196307</v>
+        <v>125.95340544447585</v>
       </c>
     </row>
     <row r="327">
       <c r="A327">
-        <v>125.54327164533368</v>
+        <v>125.54327264317173</v>
       </c>
     </row>
     <row r="328">
       <c r="A328">
-        <v>125.08404911288856</v>
+        <v>125.084050110211</v>
       </c>
     </row>
     <row r="329">
       <c r="A329">
-        <v>124.64441604814344</v>
+        <v>124.64441703170731</v>
       </c>
     </row>
     <row r="330">
       <c r="A330">
-        <v>124.29046663936603</v>
+        <v>124.29046759715919</v>
       </c>
     </row>
     <row r="331">
       <c r="A331">
-        <v>123.96958354801352</v>
+        <v>123.96958449416626</v>
       </c>
     </row>
     <row r="332">
       <c r="A332">
-        <v>123.58809680880192</v>
+        <v>123.58809776024529</v>
       </c>
     </row>
     <row r="333">
       <c r="A333">
-        <v>123.15145177849222</v>
+        <v>123.1514527464027</v>
       </c>
     </row>
     <row r="334">
       <c r="A334">
-        <v>122.78242570037681</v>
+        <v>122.78242664793028</v>
       </c>
     </row>
     <row r="335">
       <c r="A335">
-        <v>122.40002259329917</v>
+        <v>122.40002352450442</v>
       </c>
     </row>
     <row r="336">
       <c r="A336">
-        <v>122.08901474920222</v>
+        <v>122.08901563376776</v>
       </c>
     </row>
     <row r="337">
       <c r="A337">
-        <v>121.82205276524992</v>
+        <v>121.82205366855378</v>
       </c>
     </row>
     <row r="338">
       <c r="A338">
-        <v>121.48690729526456</v>
+        <v>121.48690818920781</v>
       </c>
     </row>
     <row r="339">
       <c r="A339">
-        <v>121.15168602772538</v>
+        <v>121.15168692413698</v>
       </c>
     </row>
     <row r="340">
       <c r="A340">
-        <v>120.77067997262799</v>
+        <v>120.77068085501307</v>
       </c>
     </row>
     <row r="341">
       <c r="A341">
-        <v>120.40921762179838</v>
+        <v>120.40921848385449</v>
       </c>
     </row>
     <row r="342">
       <c r="A342">
-        <v>120.15951564656676</v>
+        <v>120.15951647409278</v>
       </c>
     </row>
     <row r="343">
       <c r="A343">
-        <v>119.86021552584936</v>
+        <v>119.86021633720136</v>
       </c>
     </row>
     <row r="344">
       <c r="A344">
-        <v>119.56293364536488</v>
+        <v>119.56293444347803</v>
       </c>
     </row>
     <row r="345">
       <c r="A345">
-        <v>119.2107032789566</v>
+        <v>119.21070406667519</v>
       </c>
     </row>
     <row r="346">
       <c r="A346">
-        <v>118.99744265228092</v>
+        <v>118.99744342445848</v>
       </c>
     </row>
     <row r="347">
       <c r="A347">
-        <v>118.65218562317915</v>
+        <v>118.65218637149641</v>
       </c>
     </row>
     <row r="348">
       <c r="A348">
-        <v>118.30024715249625</v>
+        <v>118.30024790595479</v>
       </c>
     </row>
     <row r="349">
       <c r="A349">
-        <v>118.02856359755933</v>
+        <v>118.0285643672139</v>
       </c>
     </row>
     <row r="350">
       <c r="A350">
-        <v>117.75676578165691</v>
+        <v>117.75676654289785</v>
       </c>
     </row>
     <row r="351">
       <c r="A351">
-        <v>117.47768167479892</v>
+        <v>117.47768242259271</v>
       </c>
     </row>
     <row r="352">
       <c r="A352">
-        <v>117.08100378969505</v>
+        <v>117.08100454371733</v>
       </c>
     </row>
     <row r="353">
       <c r="A353">
-        <v>116.78370571167272</v>
+        <v>116.78370645829546</v>
       </c>
     </row>
     <row r="354">
       <c r="A354">
-        <v>116.46916105241097</v>
+        <v>116.46916179861076</v>
       </c>
     </row>
     <row r="355">
       <c r="A355">
-        <v>116.15220678505919</v>
+        <v>116.15220752648301</v>
       </c>
     </row>
     <row r="356">
       <c r="A356">
-        <v>115.9185985522335</v>
+        <v>115.91859931122859</v>
       </c>
     </row>
     <row r="357">
       <c r="A357">
-        <v>115.64955173523974</v>
+        <v>115.64955249491213</v>
       </c>
     </row>
     <row r="358">
       <c r="A358">
-        <v>115.35780180435289</v>
+        <v>115.35780255708936</v>
       </c>
     </row>
     <row r="359">
       <c r="A359">
-        <v>114.99519053332025</v>
+        <v>114.99519129231167</v>
       </c>
     </row>
     <row r="360">
       <c r="A360">
-        <v>114.64504884783604</v>
+        <v>114.64504958559168</v>
       </c>
     </row>
     <row r="361">
       <c r="A361">
-        <v>114.3712052376512</v>
+        <v>114.37120602883286</v>
       </c>
     </row>
     <row r="362">
       <c r="A362">
-        <v>114.22020571730205</v>
+        <v>114.2202065854969</v>
       </c>
     </row>
     <row r="363">
       <c r="A363">
-        <v>113.93866732270527</v>
+        <v>113.93866819541709</v>
       </c>
     </row>
     <row r="364">
       <c r="A364">
-        <v>113.68315198106862</v>
+        <v>113.68315291688812</v>
       </c>
     </row>
     <row r="365">
       <c r="A365">
-        <v>113.52392876456099</v>
+        <v>113.52392968516163</v>
       </c>
     </row>
     <row r="366">
       <c r="A366">
-        <v>113.3306478784251</v>
+        <v>113.33064882887187</v>
       </c>
     </row>
     <row r="367">
       <c r="A367">
-        <v>113.16869462437347</v>
+        <v>113.16869556957779</v>
       </c>
     </row>
     <row r="368">
       <c r="A368">
-        <v>112.97751968044096</v>
+        <v>112.97752065894535</v>
       </c>
     </row>
     <row r="369">
       <c r="A369">
-        <v>112.94343604043935</v>
+        <v>112.94343702607429</v>
       </c>
     </row>
     <row r="370">
       <c r="A370">
-        <v>112.7956872776726</v>
+        <v>112.79568828424145</v>
       </c>
     </row>
     <row r="371">
       <c r="A371">
-        <v>112.72586879644552</v>
+        <v>112.72586979191567</v>
       </c>
     </row>
     <row r="372">
       <c r="A372">
-        <v>112.56436247372619</v>
+        <v>112.5643634023215</v>
       </c>
     </row>
     <row r="373">
       <c r="A373">
-        <v>112.3624664716581</v>
+        <v>112.36246743203134</v>
       </c>
     </row>
     <row r="374">
       <c r="A374">
-        <v>112.14387996935221</v>
+        <v>112.14388094193185</v>
       </c>
     </row>
     <row r="375">
       <c r="A375">
-        <v>111.90533401001194</v>
+        <v>111.9053349570886</v>
       </c>
     </row>
     <row r="376">
       <c r="A376">
-        <v>111.63134643409509</v>
+        <v>111.63134741117344</v>
       </c>
     </row>
     <row r="377">
       <c r="A377">
-        <v>111.50354544276198</v>
+        <v>111.50354639787878</v>
       </c>
     </row>
     <row r="378">
       <c r="A378">
-        <v>111.31218905377544</v>
+        <v>111.31219000815545</v>
       </c>
     </row>
     <row r="379">
       <c r="A379">
-        <v>111.13636583912795</v>
+        <v>111.13636679550127</v>
       </c>
     </row>
     <row r="380">
       <c r="A380">
-        <v>110.92925868822147</v>
+        <v>110.92925964458023</v>
       </c>
     </row>
     <row r="381">
       <c r="A381">
-        <v>110.70091418783737</v>
+        <v>110.70091515177494</v>
       </c>
     </row>
     <row r="382">
       <c r="A382">
-        <v>110.4452303726864</v>
+        <v>110.44523134017072</v>
       </c>
     </row>
     <row r="383">
       <c r="A383">
-        <v>110.22235941588616</v>
+        <v>110.22236039439072</v>
       </c>
     </row>
     <row r="384">
       <c r="A384">
-        <v>110.032327325407</v>
+        <v>110.03232833812649</v>
       </c>
     </row>
     <row r="385">
       <c r="A385">
-        <v>109.82816792749929</v>
+        <v>109.82816890362248</v>
       </c>
     </row>
     <row r="386">
       <c r="A386">
-        <v>109.65436276905717</v>
+        <v>109.65436379109256</v>
       </c>
     </row>
     <row r="387">
       <c r="A387">
-        <v>109.43161059505086</v>
+        <v>109.4316116102851</v>
       </c>
     </row>
     <row r="388">
       <c r="A388">
-        <v>109.24743110138905</v>
+        <v>109.24743207059912</v>
       </c>
     </row>
     <row r="389">
       <c r="A389">
-        <v>109.11310845387248</v>
+        <v>109.11310939183295</v>
       </c>
     </row>
     <row r="390">
       <c r="A390">
-        <v>109.03570986728026</v>
+        <v>109.03571076377726</v>
       </c>
     </row>
     <row r="391">
       <c r="A391">
-        <v>108.92114806450033</v>
+        <v>108.92114894048936</v>
       </c>
     </row>
     <row r="392">
       <c r="A392">
-        <v>108.75800188265204</v>
+        <v>108.75800272228589</v>
       </c>
     </row>
     <row r="393">
       <c r="A393">
-        <v>108.57006035986419</v>
+        <v>108.57006123291305</v>
       </c>
     </row>
     <row r="394">
       <c r="A394">
-        <v>108.34585786817365</v>
+        <v>108.34585875546918</v>
       </c>
     </row>
     <row r="395">
       <c r="A395">
-        <v>108.14480976841986</v>
+        <v>108.14481063389151</v>
       </c>
     </row>
     <row r="396">
       <c r="A396">
-        <v>107.83691293443601</v>
+        <v>107.83691379828937</v>
       </c>
     </row>
     <row r="397">
       <c r="A397">
-        <v>107.58555109747672</v>
+        <v>107.58555195509574</v>
       </c>
     </row>
     <row r="398">
       <c r="A398">
-        <v>107.44507312376849</v>
+        <v>107.44507395487096</v>
       </c>
     </row>
     <row r="399">
       <c r="A399">
-        <v>107.29157327965267</v>
+        <v>107.29157410544137</v>
       </c>
     </row>
     <row r="400">
       <c r="A400">
-        <v>107.19134525124966</v>
+        <v>107.19134607811483</v>
       </c>
     </row>
     <row r="401">
       <c r="A401">
-        <v>106.95593062711809</v>
+        <v>106.9559314653842</v>
       </c>
     </row>
     <row r="402">
       <c r="A402">
-        <v>106.72706023203187</v>
+        <v>106.72706110043549</v>
       </c>
     </row>
     <row r="403">
       <c r="A403">
-        <v>106.5101508736921</v>
+        <v>106.51015175592104</v>
       </c>
     </row>
     <row r="404">
       <c r="A404">
-        <v>106.29720763701374</v>
+        <v>106.29720851972408</v>
       </c>
     </row>
     <row r="405">
       <c r="A405">
-        <v>106.07956046333426</v>
+        <v>106.079561340784</v>
       </c>
     </row>
     <row r="406">
       <c r="A406">
-        <v>105.83458719654178</v>
+        <v>105.83458806178547</v>
       </c>
     </row>
     <row r="407">
       <c r="A407">
-        <v>105.61081294663759</v>
+        <v>105.61081380647396</v>
       </c>
     </row>
     <row r="408">
       <c r="A408">
-        <v>105.46673747556272</v>
+        <v>105.46673829567783</v>
       </c>
     </row>
     <row r="409">
       <c r="A409">
-        <v>105.33634788296712</v>
+        <v>105.3363487128947</v>
       </c>
     </row>
     <row r="410">
       <c r="A410">
-        <v>105.1488156981131</v>
+        <v>105.14881653169532</v>
       </c>
     </row>
     <row r="411">
       <c r="A411">
-        <v>105.1017293605213</v>
+        <v>105.10173024226185</v>
       </c>
     </row>
     <row r="412">
       <c r="A412">
-        <v>104.88599713486748</v>
+        <v>104.88599802201175</v>
       </c>
     </row>
     <row r="413">
       <c r="A413">
-        <v>104.76498416152255</v>
+        <v>104.76498509474278</v>
       </c>
     </row>
     <row r="414">
       <c r="A414">
-        <v>104.65746777636535</v>
+        <v>104.65746870445385</v>
       </c>
     </row>
     <row r="415">
       <c r="A415">
-        <v>104.61599036632305</v>
+        <v>104.61599128740986</v>
       </c>
     </row>
     <row r="416">
       <c r="A416">
-        <v>104.48630578356466</v>
+        <v>104.48630669713806</v>
       </c>
     </row>
     <row r="417">
       <c r="A417">
-        <v>104.34417704696838</v>
+        <v>104.34417794508877</v>
       </c>
     </row>
     <row r="418">
       <c r="A418">
-        <v>104.14689830021121</v>
+        <v>104.14689920035939</v>
       </c>
     </row>
     <row r="419">
       <c r="A419">
-        <v>103.94750689898002</v>
+        <v>103.94750779114905</v>
       </c>
     </row>
     <row r="420">
       <c r="A420">
-        <v>103.81884753842196</v>
+        <v>103.81884842990259</v>
       </c>
     </row>
     <row r="421">
       <c r="A421">
-        <v>103.60421332122445</v>
+        <v>103.60421420512782</v>
       </c>
     </row>
     <row r="422">
       <c r="A422">
-        <v>103.48038472847463</v>
+        <v>103.48038560997773</v>
       </c>
     </row>
     <row r="423">
       <c r="A423">
-        <v>103.2757382597148</v>
+        <v>103.27573915156739</v>
       </c>
     </row>
     <row r="424">
       <c r="A424">
-        <v>103.08582181135269</v>
+        <v>103.08582267557698</v>
       </c>
     </row>
     <row r="425">
       <c r="A425">
-        <v>102.87214240919903</v>
+        <v>102.87214326429651</v>
       </c>
     </row>
     <row r="426">
       <c r="A426">
-        <v>102.69697425786566</v>
+        <v>102.69697508966699</v>
       </c>
     </row>
     <row r="427">
       <c r="A427">
-        <v>102.5207906089355</v>
+        <v>102.52079140713512</v>
       </c>
     </row>
     <row r="428">
       <c r="A428">
-        <v>102.40394193295548</v>
+        <v>102.40394273289567</v>
       </c>
     </row>
     <row r="429">
       <c r="A429">
-        <v>102.27766387092882</v>
+        <v>102.27766471829828</v>
       </c>
     </row>
     <row r="430">
       <c r="A430">
-        <v>102.10161075315581</v>
+        <v>102.10161161463537</v>
       </c>
     </row>
     <row r="431">
       <c r="A431">
-        <v>101.87859117825253</v>
+        <v>101.87859205184387</v>
       </c>
     </row>
     <row r="432">
       <c r="A432">
-        <v>101.74518694673689</v>
+        <v>101.74518780654498</v>
       </c>
     </row>
     <row r="433">
       <c r="A433">
-        <v>101.58379242369527</v>
+        <v>101.583793271486</v>
       </c>
     </row>
     <row r="434">
       <c r="A434">
-        <v>101.38507295768504</v>
+        <v>101.38507379799066</v>
       </c>
     </row>
     <row r="435">
       <c r="A435">
-        <v>101.20353987606899</v>
+        <v>101.20354072790856</v>
       </c>
     </row>
     <row r="436">
       <c r="A436">
-        <v>100.98962560881692</v>
+        <v>100.9896264529215</v>
       </c>
     </row>
     <row r="437">
       <c r="A437">
-        <v>100.73664605365666</v>
+        <v>100.73664686818135</v>
       </c>
     </row>
     <row r="438">
       <c r="A438">
-        <v>100.46785854935453</v>
+        <v>100.46785934519616</v>
       </c>
     </row>
     <row r="439">
       <c r="A439">
-        <v>100.25053265910587</v>
+        <v>100.25053343195962</v>
       </c>
     </row>
     <row r="440">
       <c r="A440">
-        <v>99.990492710222796</v>
+        <v>99.990493487177588</v>
       </c>
     </row>
     <row r="441">
       <c r="A441">
-        <v>99.795497325046554</v>
+        <v>99.795498136688892</v>
       </c>
     </row>
     <row r="442">
       <c r="A442">
-        <v>99.563601353673292</v>
+        <v>99.563602163996123</v>
       </c>
     </row>
     <row r="443">
       <c r="A443">
-        <v>99.299910999281806</v>
+        <v>99.299911801702237</v>
       </c>
     </row>
     <row r="444">
       <c r="A444">
-        <v>99.022745588484668</v>
+        <v>99.022746388272367</v>
       </c>
     </row>
     <row r="445">
       <c r="A445">
-        <v>98.769775039407705</v>
+        <v>98.769775834870956</v>
       </c>
     </row>
     <row r="446">
       <c r="A446">
-        <v>98.532099832691785</v>
+        <v>98.532100631206276</v>
       </c>
     </row>
     <row r="447">
       <c r="A447">
-        <v>98.267462350530138</v>
+        <v>98.267463136688292</v>
       </c>
     </row>
     <row r="448">
       <c r="A448">
-        <v>97.991061517247374</v>
+        <v>97.991062302235292</v>
       </c>
     </row>
     <row r="449">
       <c r="A449">
-        <v>97.706158500551311</v>
+        <v>97.706159280457655</v>
       </c>
     </row>
     <row r="450">
       <c r="A450">
-        <v>97.426591589143115</v>
+        <v>97.426592372553685</v>
       </c>
     </row>
     <row r="451">
       <c r="A451">
-        <v>97.157433664188886</v>
+        <v>97.157434448202977</v>
       </c>
     </row>
     <row r="452">
       <c r="A452">
-        <v>96.888173564610838</v>
+        <v>96.888174357028703</v>
       </c>
     </row>
     <row r="453">
       <c r="A453">
-        <v>96.607056994197663</v>
+        <v>96.607057779801977</v>
       </c>
     </row>
     <row r="454">
       <c r="A454">
-        <v>96.330102101142884</v>
+        <v>96.330102887085204</v>
       </c>
     </row>
     <row r="455">
       <c r="A455">
-        <v>96.0526318651183</v>
+        <v>96.052632652693021</v>
       </c>
     </row>
     <row r="456">
       <c r="A456">
-        <v>95.77706238984517</v>
+        <v>95.777063170393063</v>
       </c>
     </row>
     <row r="457">
       <c r="A457">
-        <v>95.503897560325711</v>
+        <v>95.503898337195224</v>
       </c>
     </row>
     <row r="458">
       <c r="A458">
-        <v>95.228237787191702</v>
+        <v>95.228238557706021</v>
       </c>
     </row>
     <row r="459">
       <c r="A459">
-        <v>94.948783095149196</v>
+        <v>94.94878386266565</v>
       </c>
     </row>
     <row r="460">
       <c r="A460">
-        <v>94.668003745351285</v>
+        <v>94.668004509679974</v>
       </c>
     </row>
     <row r="461">
       <c r="A461">
-        <v>94.387293587515003</v>
+        <v>94.387294349139566</v>
       </c>
     </row>
     <row r="462">
       <c r="A462">
-        <v>94.105419495234699</v>
+        <v>94.105420251184299</v>
       </c>
     </row>
     <row r="463">
       <c r="A463">
-        <v>93.843032845836845</v>
+        <v>93.843033597741908</v>
       </c>
     </row>
     <row r="464">
       <c r="A464">
-        <v>93.57895487180113</v>
+        <v>93.578955623968682</v>
       </c>
     </row>
   </sheetData>

</xml_diff>